<commit_message>
T5A - com os péssimos dados da aula
</commit_message>
<xml_diff>
--- a/t5a - inercia.xlsx
+++ b/t5a - inercia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Ambiente de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50DB3719-92B9-4C06-B160-14DE69F2CC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3405DFD-E868-4207-9393-19B0F000E431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D149F195-8FA2-4881-9A1D-3CD562656943}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>TD</t>
   </si>
@@ -249,6 +249,42 @@
   <si>
     <t>D</t>
   </si>
+  <si>
+    <t>T^2</t>
+  </si>
+  <si>
+    <t>Análise Estatística</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>u(m)</t>
+  </si>
+  <si>
+    <t>r^2</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>u(b)</t>
+  </si>
+  <si>
+    <t>sy</t>
+  </si>
+  <si>
+    <t>Erro</t>
+  </si>
+  <si>
+    <t>fit</t>
+  </si>
+  <si>
+    <t>resíduos</t>
+  </si>
+  <si>
+    <t>Dif relativa</t>
+  </si>
 </sst>
 </file>
 
@@ -279,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,8 +328,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -316,14 +358,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,6 +408,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -428,140 +526,142 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.3581154104544564E-2"/>
+                  <c:y val="0.16917185223969766"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'d1 == d2'!$G$2:$G$21</c:f>
+              <c:f>'d1 == d2'!$G$2:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>61.011721000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>56.991175562499997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>53.282700250000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>49.596806250000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>46.345460062500003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>42.922152249999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>39.614436000000005</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>36.844900000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>33.683514062500002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>31.222950062499997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>28.472896000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17.878098062499994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'d1 == d2'!$F$2:$F$21</c:f>
+              <c:f>'d1 == d2'!$F$2:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.8297709837333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.7401993740333336E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.6506277643333333E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2.561056154633333E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2.4714845449333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2.3819129352333331E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2.2923413255333331E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>2.2027697158333331E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>2.1131981061333335E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>2.0236264964333332E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9340548867333336E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.4861968382333331E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -901,6 +1001,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Resíduos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -939,9 +1064,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>I'(T2)</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -966,138 +1088,90 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'d1 == d2'!$G$2:$G$21</c:f>
+              <c:f>'d1 == d2'!$S$4:$S$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>61.011721000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>56.991175562499997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>53.282700250000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>49.596806250000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>46.345460062500003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>42.922152249999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>39.614436000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>36.844900000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>33.683514062500002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>31.222950062499997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>28.472896000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>17.878098062499994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'d1 == d2'!$F$2:$F$21</c:f>
+              <c:f>'d1 == d2'!$U$4:$U$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-6.3197452470895032E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-3.2149835858930054E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-1.0464545234253886E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.0543289934390743E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.8514381269617297E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3.1644443815413009E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4.1306677168955613E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3.4823119763385812E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4.0095339534415575E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2.4342402097853391E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1.7274372693437678E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>-1.1273219271339362E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,7 +1179,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CADC-4E85-8574-D4D5606F433B}"/>
+              <c16:uniqueId val="{00000000-6F52-449B-B11F-2140EEAC2596}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1117,13 +1191,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149293199"/>
-        <c:axId val="149296111"/>
+        <c:axId val="256949551"/>
+        <c:axId val="256946223"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149293199"/>
+        <c:axId val="256949551"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1161,25 +1236,38 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>T</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="30000">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>2</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t> (s</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="30000">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>2</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="800">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1249,12 +1337,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149296111"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="256946223"/>
+        <c:crossesAt val="-1000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149296111"/>
+        <c:axId val="256946223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,7 +1383,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>I'</a:t>
+                  <a:t>Resíduos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1366,7 +1454,339 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149293199"/>
+        <c:crossAx val="256949551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>I'(T^2)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'d1 != d2'!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>57.744801000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.100692249999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.761156</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.783760250000014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.821444000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56.776225000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.24435600000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'d1 != d2'!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.1526139755433336E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1536488217933333E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1543387192933335E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1550286167933331E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1557185142933333E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1564084117933336E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1570983092933325E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D081-4504-93E2-51578FA61572}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="441814911"/>
+        <c:axId val="441816575"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="441814911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441816575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="441816575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441814911"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1502,6 +1922,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2534,20 +2994,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2572,6 +3548,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF48CE9A-242E-DFFF-82E3-DEA46A7B0A86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2579,29 +3591,27 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9289B86D-2932-4CEB-A4D1-3A08BEB1A034}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{733D4E64-1A91-913F-B04C-EF9ADA75FFAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2915,485 +3925,875 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA1F82D-724E-4007-ACEE-899E5FEDB6AF}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="12" width="8.88671875" style="2"/>
+    <col min="13" max="13" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:21" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3">
-        <f>(B2+C2)/2</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <f>(1/(4*PI()^2))*D2^2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <f>J2*L2^2+J3*L3^2+(J4*L4^2)/12</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7.8040000000000003</v>
+      </c>
+      <c r="C2" s="4">
+        <v>7.8120000000000003</v>
+      </c>
+      <c r="D2" s="5">
+        <f>AVERAGE(AVERAGE(B2:B3),AVERAGE(C2:C3))</f>
+        <v>7.8109999999999999</v>
+      </c>
+      <c r="E2" s="5">
+        <f>($J$8/(4*PI()^2))*D2^2</f>
+        <v>1.8303950788222979E-2</v>
+      </c>
+      <c r="F2" s="5">
+        <f>A2*$J$3^2+A2*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.8297709837333332E-2</v>
+      </c>
+      <c r="G2" s="5">
         <f>D2^2</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
+        <v>61.011721000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1">
+        <v>7.8140000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7.8140000000000001</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="3"/>
+      <c r="J3" s="1">
+        <v>0.21243999999999999</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="R3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D21" si="0">(B3+C3)/2</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E21" si="1">(1/(4*PI()^2))*D3^2</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" ref="F3:F21" si="2">J3*L3^2+J4*L4^2+(J5*L5^2)/12</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G21" si="3">D3^2</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="s">
+    <row r="4" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>0.26</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7.548</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7.5540000000000003</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4" si="0">AVERAGE(AVERAGE(B4:B5),AVERAGE(C4:C5))</f>
+        <v>7.5492499999999998</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4" si="1">($J$8/(4*PI()^2))*D4^2</f>
+        <v>1.7097758525103333E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F25" si="2">A4*$J$3^2+A4*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.7401993740333336E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <f>D4^2</f>
+        <v>56.991175562499997</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="3"/>
+      <c r="J4" s="1">
+        <v>0.21081</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="array" ref="M4:N6">LINEST(R4:R15,S4:S15,1,1)</f>
+        <v>3.0000712138939629E-4</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1.0625733573819303E-2</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="2">
+        <f>F2</f>
+        <v>2.8297709837333332E-2</v>
+      </c>
+      <c r="S4" s="2">
+        <f>G2</f>
+        <v>61.011721000000001</v>
+      </c>
+      <c r="T4" s="2">
+        <f>S4*$M$4+$N$4</f>
+        <v>2.8929684362042282E-2</v>
+      </c>
+      <c r="U4" s="2">
+        <f>R4-T4</f>
+        <v>-6.3197452470895032E-4</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
+    <row r="5" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1">
+        <v>7.5469999999999997</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.548</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="I5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.13222</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.1816725821147807E-5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>5.1083894415390534E-4</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="2">
+        <f>F4</f>
+        <v>2.7401993740333336E-2</v>
+      </c>
+      <c r="S5" s="2">
+        <f>G4</f>
+        <v>56.991175562499997</v>
+      </c>
+      <c r="T5" s="2">
+        <f t="shared" ref="T5:T15" si="3">S5*$M$4+$N$4</f>
+        <v>2.7723492098922636E-2</v>
+      </c>
+      <c r="U5" s="2">
+        <f t="shared" ref="U5:U15" si="4">R5-T5</f>
+        <v>-3.2149835858930054E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7.2939999999999996</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7.306</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" ref="D6" si="5">AVERAGE(AVERAGE(B6:B7),AVERAGE(C6:C7))</f>
+        <v>7.2995000000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ref="E6" si="6">($J$8/(4*PI()^2))*D6^2</f>
+        <v>1.5985189521856569E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" ref="F6:F25" si="7">A6*$J$3^2+A6*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.6506277643333333E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <f>D6^2</f>
+        <v>53.282700250000005</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.98472275083186844</v>
+      </c>
+      <c r="N6" s="1">
+        <v>4.971758443382163E-4</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" s="2">
+        <f>F6</f>
+        <v>2.6506277643333333E-2</v>
+      </c>
+      <c r="S6" s="2">
+        <f>G6</f>
+        <v>53.282700250000005</v>
+      </c>
+      <c r="T6" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="3"/>
+        <v>2.6610923095675872E-2</v>
+      </c>
+      <c r="U6" s="2">
+        <f t="shared" si="4"/>
+        <v>-1.0464545234253886E-4</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1">
+        <v>7.2990000000000004</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.2990000000000004</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="R7" s="2">
+        <f>F8</f>
+        <v>2.561056154633333E-2</v>
+      </c>
+      <c r="S7" s="2">
+        <f>G8</f>
+        <v>49.596806250000007</v>
+      </c>
+      <c r="T7" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.5505128646989422E-2</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0543289934390743E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>0.24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.0380000000000003</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.0439999999999996</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" ref="D8" si="8">AVERAGE(AVERAGE(B8:B9),AVERAGE(C8:C9))</f>
+        <v>7.0425000000000004</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ref="E8" si="9">($J$8/(4*PI()^2))*D8^2</f>
+        <v>1.4879395073170121E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:F25" si="10">A8*$J$3^2+A8*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.561056154633333E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <f>D8^2</f>
+        <v>49.596806250000007</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="1">
+        <f>M4*4*PI()*PI()</f>
+        <v>1.184380642249174E-2</v>
+      </c>
+      <c r="R8" s="2">
+        <f>F10</f>
+        <v>2.4714845449333334E-2</v>
+      </c>
+      <c r="S8" s="2">
+        <f>G10</f>
+        <v>46.345460062500003</v>
+      </c>
+      <c r="T8" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.4529701636637161E-2</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="4"/>
+        <v>1.8514381269617297E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="1">
+        <v>7.0419999999999998</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7.0460000000000003</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="I9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="8">
+        <f>ABS(J8-0.02289)/0.02289</f>
+        <v>0.48257726419870078</v>
+      </c>
+      <c r="R9" s="2">
+        <f>F12</f>
+        <v>2.3819129352333331E-2</v>
+      </c>
+      <c r="S9" s="2">
+        <f>G12</f>
+        <v>42.922152249999996</v>
+      </c>
+      <c r="T9" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.35026849141792E-2</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" si="4"/>
+        <v>3.1644443815413009E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6.8120000000000003</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.8079999999999998</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" ref="D10" si="11">AVERAGE(AVERAGE(B10:B11),AVERAGE(C10:C11))</f>
+        <v>6.8077500000000004</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" ref="E10" si="12">($J$8/(4*PI()^2))*D10^2</f>
+        <v>1.3903968062817856E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" ref="F10:F25" si="13">A10*$J$3^2+A10*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.4714845449333334E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <f>D10^2</f>
+        <v>46.345460062500003</v>
+      </c>
+      <c r="R10" s="2">
+        <f>F14</f>
+        <v>2.2923413255333331E-2</v>
+      </c>
+      <c r="S10" s="2">
+        <f>G14</f>
+        <v>39.614436000000005</v>
+      </c>
+      <c r="T10" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.2510346483643775E-2</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="4"/>
+        <v>4.1306677168955613E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1">
+        <v>6.81</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.8010000000000002</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="R11" s="2">
+        <f>F16</f>
+        <v>2.2027697158333331E-2</v>
+      </c>
+      <c r="S11" s="2">
+        <f>G16</f>
+        <v>36.844900000000003</v>
+      </c>
+      <c r="T11" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.1679465960699473E-2</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="4"/>
+        <v>3.4823119763385812E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6.5549999999999997</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.5469999999999997</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" ref="D12" si="14">AVERAGE(AVERAGE(B12:B13),AVERAGE(C12:C13))</f>
+        <v>6.5514999999999999</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" ref="E12" si="15">($J$8/(4*PI()^2))*D12^2</f>
+        <v>1.2876951340359898E-2</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" ref="F12:F25" si="16">A12*$J$3^2+A12*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.3819129352333331E-2</v>
+      </c>
+      <c r="G12" s="5">
+        <f>D12^2</f>
+        <v>42.922152249999996</v>
+      </c>
+      <c r="R12" s="2">
+        <f>F18</f>
+        <v>2.1131981061333335E-2</v>
+      </c>
+      <c r="S12" s="2">
+        <f>G18</f>
+        <v>33.683514062500002</v>
+      </c>
+      <c r="T12" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.073102766598918E-2</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" si="4"/>
+        <v>4.0095339534415575E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1">
+        <v>6.5549999999999997</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6.5490000000000004</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="R13" s="2">
+        <f>F20</f>
+        <v>2.0236264964333332E-2</v>
+      </c>
+      <c r="S13" s="2">
+        <f>G20</f>
+        <v>31.222950062499997</v>
+      </c>
+      <c r="T13" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.9992840943354798E-2</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="4"/>
+        <v>2.4342402097853391E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6.2960000000000003</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6.2919999999999998</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" ref="D14" si="17">AVERAGE(AVERAGE(B14:B15),AVERAGE(C14:C15))</f>
+        <v>6.2940000000000005</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" ref="E14" si="18">($J$8/(4*PI()^2))*D14^2</f>
+        <v>1.1884612909824472E-2</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" ref="F14:F25" si="19">A14*$J$3^2+A14*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.2923413255333331E-2</v>
+      </c>
+      <c r="G14" s="5">
+        <f>D14^2</f>
+        <v>39.614436000000005</v>
+      </c>
+      <c r="R14" s="2">
+        <f>F22</f>
+        <v>1.9340548867333336E-2</v>
+      </c>
+      <c r="S14" s="2">
+        <f>G22</f>
+        <v>28.472896000000002</v>
+      </c>
+      <c r="T14" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.9167805140398959E-2</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="4"/>
+        <v>1.7274372693437678E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="1">
+        <v>6.298</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="R15" s="2">
+        <f>F24</f>
+        <v>1.4861968382333331E-2</v>
+      </c>
+      <c r="S15" s="2">
+        <f>G24</f>
+        <v>17.878098062499994</v>
+      </c>
+      <c r="T15" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.5989290309467268E-2</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="4"/>
+        <v>-1.1273219271339362E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6.0720000000000001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6.069</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" ref="D16" si="20">AVERAGE(AVERAGE(B16:B17),AVERAGE(C16:C17))</f>
+        <v>6.07</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" ref="E16" si="21">($J$8/(4*PI()^2))*D16^2</f>
+        <v>1.1053732386880169E-2</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" ref="F16:F25" si="22">A16*$J$3^2+A16*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.2027697158333331E-2</v>
+      </c>
+      <c r="G16" s="5">
+        <f>D16^2</f>
+        <v>36.844900000000003</v>
+      </c>
+      <c r="R16" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="1">
+        <v>6.0730000000000004</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6.0659999999999998</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="R17" s="9"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5.8070000000000004</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5.8019999999999996</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" ref="D18" si="23">AVERAGE(AVERAGE(B18:B19),AVERAGE(C18:C19))</f>
+        <v>5.80375</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" ref="E18" si="24">($J$8/(4*PI()^2))*D18^2</f>
+        <v>1.0105294092169875E-2</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" ref="F18:F25" si="25">A18*$J$3^2+A18*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.1131981061333335E-2</v>
+      </c>
+      <c r="G18" s="5">
+        <f>D18^2</f>
+        <v>33.683514062500002</v>
+      </c>
+      <c r="R18" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="1">
+        <v>5.8070000000000004</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5.7990000000000004</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5.5910000000000002</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5.5839999999999996</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" ref="D20" si="26">AVERAGE(AVERAGE(B20:B21),AVERAGE(C20:C21))</f>
+        <v>5.5877499999999998</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" ref="E20" si="27">($J$8/(4*PI()^2))*D20^2</f>
+        <v>9.3671073695354955E-3</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" ref="F20:F25" si="28">A20*$J$3^2+A20*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>2.0236264964333332E-2</v>
+      </c>
+      <c r="G20" s="5">
+        <f>D20^2</f>
+        <v>31.222950062499997</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1">
+        <v>5.5919999999999996</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5.5839999999999996</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>0.17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5.3390000000000004</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5.3310000000000004</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" ref="D22" si="29">AVERAGE(AVERAGE(B22:B23),AVERAGE(C22:C23))</f>
+        <v>5.3360000000000003</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" ref="E22" si="30">($J$8/(4*PI()^2))*D22^2</f>
+        <v>8.5420715665796565E-3</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" ref="F22:F25" si="31">A22*$J$3^2+A22*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>1.9340548867333336E-2</v>
+      </c>
+      <c r="G22" s="5">
+        <f>D22^2</f>
+        <v>28.472896000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="1">
+        <v>5.343</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5.3310000000000004</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4.2329999999999997</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4.2249999999999996</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" ref="D24" si="32">AVERAGE(AVERAGE(B24:B25),AVERAGE(C24:C25))</f>
+        <v>4.2282499999999992</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" ref="E24" si="33">($J$8/(4*PI()^2))*D24^2</f>
+        <v>5.3635567356479664E-3</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" ref="F24:F25" si="34">A24*$J$3^2+A24*$J$4^2+($J$5*$J$6^2)/12</f>
+        <v>1.4861968382333331E-2</v>
+      </c>
+      <c r="G24" s="5">
+        <f>D24^2</f>
+        <v>17.878098062499994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="1">
+        <v>4.2309999999999999</v>
+      </c>
+      <c r="C25" s="1">
+        <v>4.2240000000000002</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="61">
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A14:A15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -3402,648 +4802,386 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322AEA10-24EE-40F7-8525-64347259AD68}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="8" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="11.33203125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <f>B2-N2</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <f>N4-C2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3">
+    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <f>B2-$P$2</f>
+        <v>0.11049999999999999</v>
+      </c>
+      <c r="B2" s="1">
+        <f>$N$5-C2</f>
+        <v>0.376</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7.6029999999999998</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7.5949999999999998</v>
+      </c>
+      <c r="F2" s="1">
         <f>(D2+E2)/2</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <f>(1/(4*PI()^2))*F2^2</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <f>L2*N2^2+L3*N3^2+(L4*N4^2)/12</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
+        <v>7.5990000000000002</v>
+      </c>
+      <c r="G2" s="1">
+        <f>('d1 == d2'!$J$8/(4*PI()^2))*F2^2</f>
+        <v>1.7323851523213533E-2</v>
+      </c>
+      <c r="H2" s="1">
+        <f>B2*$N$2^2+C2*$N$3^2+($N$4*$N$5^2)/12</f>
+        <v>3.1526139755433336E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <f>ABS(G2-H2)/H2*100</f>
+        <v>45.049245934945539</v>
+      </c>
+      <c r="J2" s="1">
         <f>F2^2</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="5" t="s">
+        <v>57.744801000000002</v>
+      </c>
+      <c r="K2" s="2">
+        <f>G2+($N$2+$N$3+$N$4)*A2^2</f>
+        <v>2.4106279090713532E-2</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="1">
+        <v>0.21243999999999999</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="3"/>
+      <c r="P2" s="1">
+        <v>0.26550000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <f t="shared" ref="A3:A21" si="0">B3-N3</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="3">
-        <f t="shared" ref="B3:B21" si="1">N5-C3</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3">
-        <f t="shared" ref="F3:F21" si="2">(D3+E3)/2</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G21" si="3">(1/(4*PI()^2))*F3^2</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H21" si="4">L3*N3^2+L4*N4^2+(L5*N5^2)/12</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <f t="shared" ref="I3:I21" si="5">F3^2</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="5" t="s">
+    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A8" si="0">B3-$P$2</f>
+        <v>0.1255</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B8" si="1">$N$5-C3</f>
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7.5609999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7.5519999999999996</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F8" si="2">(D3+E3)/2</f>
+        <v>7.5564999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <f>('d1 == d2'!$J$8/(4*PI()^2))*F3^2</f>
+        <v>1.7130614311264308E-2</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H8" si="3">B3*$N$2^2+C3*$N$3^2+($N$4*$N$5^2)/12</f>
+        <v>3.1536488217933333E-2</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I8" si="4">ABS(G3-H3)/H3*100</f>
+        <v>45.680019306896305</v>
+      </c>
+      <c r="J3" s="1">
+        <f>F3^2</f>
+        <v>57.100692249999994</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K8" si="5">G3+($N$2+$N$3+$N$4)*A3^2</f>
+        <v>2.587940567876431E-2</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="1">
+        <v>0.21081</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="P3" s="1">
+        <v>0.26550000000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B4" s="3">
+        <v>0.13550000000000001</v>
+      </c>
+      <c r="B4" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7.5369999999999999</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7.5309999999999997</v>
+      </c>
+      <c r="F4" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
+        <v>7.5339999999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <f>('d1 == d2'!$J$8/(4*PI()^2))*F4^2</f>
+        <v>1.7028751018294458E-2</v>
+      </c>
+      <c r="H4" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
+        <v>3.1543387192933335E-2</v>
+      </c>
+      <c r="I4" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
+        <v>46.014830575616152</v>
+      </c>
+      <c r="J4" s="1">
+        <f>F4^2</f>
+        <v>56.761156</v>
+      </c>
+      <c r="K4" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K4" s="5" t="s">
+        <v>2.7227319085794462E-2</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="1">
+        <v>0.13222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14549999999999996</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.5410000000000004</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7.53</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="2"/>
+        <v>7.5355000000000008</v>
+      </c>
+      <c r="G5" s="1">
+        <f>('d1 == d2'!$J$8/(4*PI()^2))*F5^2</f>
+        <v>1.7035532454268129E-2</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="3"/>
+        <v>3.1550286167933331E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="4"/>
+        <v>46.005141241531803</v>
+      </c>
+      <c r="J5" s="1">
+        <f>F5^2</f>
+        <v>56.783760250000014</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="5"/>
+        <v>2.879497122176812E-2</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="3"/>
+      <c r="N5" s="1">
+        <v>0.61099999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B5" s="3">
+        <v>0.15549999999999997</v>
+      </c>
+      <c r="B6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7.5439999999999996</v>
+      </c>
+      <c r="E6" s="1">
+        <v>7.532</v>
+      </c>
+      <c r="F6" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+        <v>7.5380000000000003</v>
+      </c>
+      <c r="G6" s="1">
+        <f>('d1 == d2'!$J$8/(4*PI()^2))*F6^2</f>
+        <v>1.7046837847628785E-2</v>
+      </c>
+      <c r="H6" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
+        <v>3.1557185142933333E-2</v>
+      </c>
+      <c r="I6" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
+        <v>45.981120399624366</v>
+      </c>
+      <c r="J6" s="1">
+        <f>F6^2</f>
+        <v>56.821444000000007</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.047824131512878E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B6" s="3">
+        <v>0.16549999999999998</v>
+      </c>
+      <c r="B7" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.5460000000000003</v>
+      </c>
+      <c r="E7" s="1">
+        <v>7.524</v>
+      </c>
+      <c r="F7" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <f>('d1 == d2'!$J$8/(4*PI()^2))*F7^2</f>
+        <v>1.7033271825606676E-2</v>
+      </c>
+      <c r="H7" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
+        <v>3.1564084117933336E-2</v>
+      </c>
+      <c r="I7" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
+        <v>46.035906627402781</v>
+      </c>
+      <c r="J7" s="1">
+        <f>F7^2</f>
+        <v>56.776225000000004</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.2247733993106674E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B7" s="3">
+        <v>0.17549999999999993</v>
+      </c>
+      <c r="B8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3">
+        <v>0.44099999999999995</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7.5860000000000003</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7.5460000000000003</v>
+      </c>
+      <c r="F8" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+        <v>7.5660000000000007</v>
+      </c>
+      <c r="G8" s="1">
+        <f>('d1 == d2'!$J$8/(4*PI()^2))*F8^2</f>
+        <v>1.7173714459349818E-2</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
+        <v>3.1570983092933325E-2</v>
+      </c>
+      <c r="I8" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
+        <v>45.602851806050069</v>
+      </c>
+      <c r="J8" s="1">
+        <f>F8^2</f>
+        <v>57.24435600000001</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B8" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B9" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B10" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B18" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B20" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4282329326849804E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4054,28 +5192,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C7C9C7-DDA4-41C1-9791-3ACEA0C01E4B}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4083,12 +5224,12 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1">
+      <c r="D2" s="5">
         <f>(B2+C2)/2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="5"/>
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="1"/>
@@ -4097,136 +5238,51 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
t5a - formulas corrigidas
</commit_message>
<xml_diff>
--- a/t5a - inercia.xlsx
+++ b/t5a - inercia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3405DFD-E868-4207-9393-19B0F000E431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469F9064-4C4C-4965-87AD-0DF87F0F3E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D149F195-8FA2-4881-9A1D-3CD562656943}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{D149F195-8FA2-4881-9A1D-3CD562656943}"/>
   </bookViews>
   <sheets>
     <sheet name="d1 == d2" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>TD</t>
   </si>
@@ -274,16 +274,28 @@
     <t>sy</t>
   </si>
   <si>
-    <t>Erro</t>
-  </si>
-  <si>
     <t>fit</t>
   </si>
   <si>
     <t>resíduos</t>
   </si>
   <si>
-    <t>Dif relativa</t>
+    <t>I ZZ'</t>
+  </si>
+  <si>
+    <t>I OO'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>I ZZ' (Steiner)</t>
+  </si>
+  <si>
+    <t>Erro %</t>
   </si>
 </sst>
 </file>
@@ -399,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -413,12 +425,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,7 +434,22 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -505,7 +526,7 @@
             <c:v>I'(T2)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -578,44 +599,41 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'d1 == d2'!$G$2:$G$33</c:f>
+              <c:f>'d1 == d2'!$S$5:$S$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>61.011721000000001</c:v>
+                  <c:v>56.991175562499997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.282700250000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.991175562499997</c:v>
+                  <c:v>49.596806250000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.345460062500003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.282700250000005</c:v>
+                  <c:v>42.922152249999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.614436000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49.596806250000007</c:v>
+                  <c:v>36.844900000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.683514062500002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46.345460062500003</c:v>
+                  <c:v>31.222950062499997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.472896000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.922152249999996</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>39.614436000000005</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>36.844900000000003</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>33.683514062500002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>31.222950062499997</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>28.472896000000002</c:v>
-                </c:pt>
-                <c:pt idx="22">
                   <c:v>17.878098062499994</c:v>
                 </c:pt>
               </c:numCache>
@@ -623,45 +641,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'d1 == d2'!$F$2:$F$33</c:f>
+              <c:f>'d1 == d2'!$R$5:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.8297709837333332E-2</c:v>
+                  <c:v>2.9501831704366672E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7343256704366669E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7401993740333336E-2</c:v>
+                  <c:v>2.5269331704366665E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3280056704366666E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6506277643333333E-2</c:v>
+                  <c:v>2.1375431704366666E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9555456704366665E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.561056154633333E-2</c:v>
+                  <c:v>1.7820131704366669E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6169456704366668E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4714845449333334E-2</c:v>
+                  <c:v>1.4603431704366664E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3122056704366667E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3819129352333331E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.2923413255333331E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.2027697158333331E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.1131981061333335E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.0236264964333332E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.9340548867333336E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.4861968382333331E-2</c:v>
+                  <c:v>6.9849317043666655E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1138,40 +1153,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-6.3197452470895032E-4</c:v>
+                  <c:v>-3.4057557465869137E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.2149835858930054E-4</c:v>
+                  <c:v>3.2325465109110663E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.0464545234253886E-4</c:v>
+                  <c:v>4.0893622606057167E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0543289934390743E-4</c:v>
+                  <c:v>4.7531392454988608E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8514381269617297E-4</c:v>
+                  <c:v>-7.4003183875549772E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1644443815413009E-4</c:v>
+                  <c:v>-1.2104161102678701E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1306677168955613E-4</c:v>
+                  <c:v>6.8043124830715479E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4823119763385812E-4</c:v>
+                  <c:v>-7.6317996301235314E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0095339534415575E-4</c:v>
+                  <c:v>8.9069634306878503E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4342402097853391E-4</c:v>
+                  <c:v>-6.3480889953117584E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7274372693437678E-4</c:v>
+                  <c:v>3.4916562317520092E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.1273219271339362E-3</c:v>
+                  <c:v>-1.6011752581387637E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1510,338 +1525,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>I'(T^2)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'d1 != d2'!$J$2:$J$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>57.744801000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>57.100692249999994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56.761156</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>56.783760250000014</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>56.821444000000007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>56.776225000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>57.24435600000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'d1 != d2'!$H$2:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3.1526139755433336E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.1536488217933333E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.1543387192933335E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.1550286167933331E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.1557185142933333E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.1564084117933336E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.1570983092933325E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D081-4504-93E2-51578FA61572}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="441814911"/>
-        <c:axId val="441816575"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="441814911"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="441816575"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="441816575"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="441814911"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1922,46 +1605,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2479,522 +2122,6 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3550,16 +2677,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3579,47 +2706,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{733D4E64-1A91-913F-B04C-EF9ADA75FFAF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3927,8 +3013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA1F82D-724E-4007-ACEE-899E5FEDB6AF}">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3963,7 +3049,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="12">
         <v>0.27</v>
       </c>
       <c r="B2" s="4">
@@ -3972,47 +3058,47 @@
       <c r="C2" s="4">
         <v>7.8120000000000003</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="9">
         <f>AVERAGE(AVERAGE(B2:B3),AVERAGE(C2:C3))</f>
         <v>7.8109999999999999</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="9">
         <f>($J$8/(4*PI()^2))*D2^2</f>
-        <v>1.8303950788222979E-2</v>
-      </c>
-      <c r="F2" s="5">
-        <f>A2*$J$3^2+A2*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.8297709837333332E-2</v>
-      </c>
-      <c r="G2" s="5">
+        <v>3.5048269565217699E-2</v>
+      </c>
+      <c r="F2" s="9">
+        <f>A2^2*$J$3+A2^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>3.174505670436667E-2</v>
+      </c>
+      <c r="G2" s="9">
         <f>D2^2</f>
         <v>61.011721000000001</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1">
         <v>7.8140000000000001</v>
       </c>
       <c r="C3" s="1">
         <v>7.8140000000000001</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="1">
         <v>0.21243999999999999</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
       <c r="R3" s="2" t="s">
         <v>4</v>
       </c>
@@ -4020,14 +3106,14 @@
         <v>20</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="12">
         <v>0.26</v>
       </c>
       <c r="B4" s="1">
@@ -4036,19 +3122,19 @@
       <c r="C4" s="1">
         <v>7.5540000000000003</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="9">
         <f t="shared" ref="D4" si="0">AVERAGE(AVERAGE(B4:B5),AVERAGE(C4:C5))</f>
         <v>7.5492499999999998</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="9">
         <f t="shared" ref="E4" si="1">($J$8/(4*PI()^2))*D4^2</f>
-        <v>1.7097758525103333E-2</v>
-      </c>
-      <c r="F4" s="5">
-        <f t="shared" ref="F4:F25" si="2">A4*$J$3^2+A4*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.7401993740333336E-2</v>
-      </c>
-      <c r="G4" s="5">
+        <v>3.2738661542642725E-2</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F25" si="2">A4^2*$J$3+A4^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>2.9501831704366672E-2</v>
+      </c>
+      <c r="G4" s="9">
         <f>D4^2</f>
         <v>56.991175562499997</v>
       </c>
@@ -4063,17 +3149,17 @@
       </c>
       <c r="M4" s="1">
         <f t="array" ref="M4:N6">LINEST(R4:R15,S4:S15,1,1)</f>
-        <v>3.0000712138939629E-4</v>
+        <v>5.7445141672397176E-4</v>
       </c>
       <c r="N4" s="1">
-        <v>1.0625733573819303E-2</v>
+        <v>-3.2691553033851635E-3</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R4" s="2">
         <f>F2</f>
-        <v>2.8297709837333332E-2</v>
+        <v>3.174505670436667E-2</v>
       </c>
       <c r="S4" s="2">
         <f>G2</f>
@@ -4081,25 +3167,25 @@
       </c>
       <c r="T4" s="2">
         <f>S4*$M$4+$N$4</f>
-        <v>2.8929684362042282E-2</v>
+        <v>3.1779114261832539E-2</v>
       </c>
       <c r="U4" s="2">
         <f>R4-T4</f>
-        <v>-6.3197452470895032E-4</v>
+        <v>-3.4057557465869137E-5</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1">
         <v>7.5469999999999997</v>
       </c>
       <c r="C5" s="1">
         <v>7.548</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
@@ -4110,17 +3196,17 @@
         <v>23</v>
       </c>
       <c r="M5" s="1">
-        <v>1.1816725821147807E-5</v>
+        <v>1.3858191007623874E-6</v>
       </c>
       <c r="N5" s="1">
-        <v>5.1083894415390534E-4</v>
+        <v>5.9909181014831086E-5</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R5" s="2">
         <f>F4</f>
-        <v>2.7401993740333336E-2</v>
+        <v>2.9501831704366672E-2</v>
       </c>
       <c r="S5" s="2">
         <f>G4</f>
@@ -4128,15 +3214,15 @@
       </c>
       <c r="T5" s="2">
         <f t="shared" ref="T5:T15" si="3">S5*$M$4+$N$4</f>
-        <v>2.7723492098922636E-2</v>
+        <v>2.9469506239257561E-2</v>
       </c>
       <c r="U5" s="2">
         <f t="shared" ref="U5:U15" si="4">R5-T5</f>
-        <v>-3.2149835858930054E-4</v>
+        <v>3.2325465109110663E-5</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="12">
         <v>0.25</v>
       </c>
       <c r="B6" s="1">
@@ -4145,19 +3231,19 @@
       <c r="C6" s="1">
         <v>7.306</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="9">
         <f t="shared" ref="D6" si="5">AVERAGE(AVERAGE(B6:B7),AVERAGE(C6:C7))</f>
         <v>7.2995000000000001</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="9">
         <f t="shared" ref="E6" si="6">($J$8/(4*PI()^2))*D6^2</f>
-        <v>1.5985189521856569E-2</v>
-      </c>
-      <c r="F6" s="5">
-        <f t="shared" ref="F6:F25" si="7">A6*$J$3^2+A6*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.6506277643333333E-2</v>
-      </c>
-      <c r="G6" s="5">
+        <v>3.0608322645491227E-2</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" ref="F6:F25" si="7">A6^2*$J$3+A6^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>2.7343256704366669E-2</v>
+      </c>
+      <c r="G6" s="9">
         <f>D6^2</f>
         <v>53.282700250000005</v>
       </c>
@@ -4171,17 +3257,17 @@
         <v>24</v>
       </c>
       <c r="M6" s="1">
-        <v>0.98472275083186844</v>
+        <v>0.99994180559905266</v>
       </c>
       <c r="N6" s="1">
-        <v>4.971758443382163E-4</v>
+        <v>5.8306826438208972E-5</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="R6" s="2">
         <f>F6</f>
-        <v>2.6506277643333333E-2</v>
+        <v>2.7343256704366669E-2</v>
       </c>
       <c r="S6" s="2">
         <f>G6</f>
@@ -4189,28 +3275,32 @@
       </c>
       <c r="T6" s="2">
         <f t="shared" si="3"/>
-        <v>2.6610923095675872E-2</v>
+        <v>2.7339167342106063E-2</v>
       </c>
       <c r="U6" s="2">
         <f t="shared" si="4"/>
-        <v>-1.0464545234253886E-4</v>
+        <v>4.0893622606057167E-6</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1">
         <v>7.2990000000000004</v>
       </c>
       <c r="C7" s="1">
         <v>7.2990000000000004</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="N7" s="2">
+        <f>N4/M4</f>
+        <v>-5.690916948257815</v>
+      </c>
       <c r="R7" s="2">
         <f>F8</f>
-        <v>2.561056154633333E-2</v>
+        <v>2.5269331704366665E-2</v>
       </c>
       <c r="S7" s="2">
         <f>G8</f>
@@ -4218,15 +3308,15 @@
       </c>
       <c r="T7" s="2">
         <f t="shared" si="3"/>
-        <v>2.5505128646989422E-2</v>
+        <v>2.5221800311911676E-2</v>
       </c>
       <c r="U7" s="2">
         <f t="shared" si="4"/>
-        <v>1.0543289934390743E-4</v>
+        <v>4.7531392454988608E-5</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="12">
         <v>0.24</v>
       </c>
       <c r="B8" s="1">
@@ -4235,19 +3325,19 @@
       <c r="C8" s="1">
         <v>7.0439999999999996</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="9">
         <f t="shared" ref="D8" si="8">AVERAGE(AVERAGE(B8:B9),AVERAGE(C8:C9))</f>
         <v>7.0425000000000004</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="9">
         <f t="shared" ref="E8" si="9">($J$8/(4*PI()^2))*D8^2</f>
-        <v>1.4879395073170121E-2</v>
-      </c>
-      <c r="F8" s="5">
-        <f t="shared" ref="F8:F25" si="10">A8*$J$3^2+A8*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.561056154633333E-2</v>
-      </c>
-      <c r="G8" s="5">
+        <v>2.849095561529684E-2</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" ref="F8:F25" si="10">A8^2*$J$3+A8^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>2.5269331704366665E-2</v>
+      </c>
+      <c r="G8" s="9">
         <f>D8^2</f>
         <v>49.596806250000007</v>
       </c>
@@ -4256,11 +3346,11 @@
       </c>
       <c r="J8" s="1">
         <f>M4*4*PI()*PI()</f>
-        <v>1.184380642249174E-2</v>
+        <v>2.2678432922843713E-2</v>
       </c>
       <c r="R8" s="2">
         <f>F10</f>
-        <v>2.4714845449333334E-2</v>
+        <v>2.3280056704366666E-2</v>
       </c>
       <c r="S8" s="2">
         <f>G10</f>
@@ -4268,35 +3358,28 @@
       </c>
       <c r="T8" s="2">
         <f t="shared" si="3"/>
-        <v>2.4529701636637161E-2</v>
+        <v>2.3354059888242216E-2</v>
       </c>
       <c r="U8" s="2">
         <f t="shared" si="4"/>
-        <v>1.8514381269617297E-4</v>
+        <v>-7.4003183875549772E-5</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1">
         <v>7.0419999999999998</v>
       </c>
       <c r="C9" s="1">
         <v>7.0460000000000003</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="I9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="8">
-        <f>ABS(J8-0.02289)/0.02289</f>
-        <v>0.48257726419870078</v>
-      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
       <c r="R9" s="2">
         <f>F12</f>
-        <v>2.3819129352333331E-2</v>
+        <v>2.1375431704366666E-2</v>
       </c>
       <c r="S9" s="2">
         <f>G12</f>
@@ -4304,15 +3387,15 @@
       </c>
       <c r="T9" s="2">
         <f t="shared" si="3"/>
-        <v>2.35026849141792E-2</v>
+        <v>2.1387535865469345E-2</v>
       </c>
       <c r="U9" s="2">
         <f t="shared" si="4"/>
-        <v>3.1644443815413009E-4</v>
+        <v>-1.2104161102678701E-5</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="12">
         <v>0.23</v>
       </c>
       <c r="B10" s="1">
@@ -4321,25 +3404,25 @@
       <c r="C10" s="1">
         <v>6.8079999999999998</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="9">
         <f t="shared" ref="D10" si="11">AVERAGE(AVERAGE(B10:B11),AVERAGE(C10:C11))</f>
         <v>6.8077500000000004</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="9">
         <f t="shared" ref="E10" si="12">($J$8/(4*PI()^2))*D10^2</f>
-        <v>1.3903968062817856E-2</v>
-      </c>
-      <c r="F10" s="5">
-        <f t="shared" ref="F10:F25" si="13">A10*$J$3^2+A10*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.4714845449333334E-2</v>
-      </c>
-      <c r="G10" s="5">
+        <v>2.6623215191627379E-2</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" ref="F10:F25" si="13">A10^2*$J$3+A10^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>2.3280056704366666E-2</v>
+      </c>
+      <c r="G10" s="9">
         <f>D10^2</f>
         <v>46.345460062500003</v>
       </c>
       <c r="R10" s="2">
         <f>F14</f>
-        <v>2.2923413255333331E-2</v>
+        <v>1.9555456704366665E-2</v>
       </c>
       <c r="S10" s="2">
         <f>G14</f>
@@ -4347,28 +3430,28 @@
       </c>
       <c r="T10" s="2">
         <f t="shared" si="3"/>
-        <v>2.2510346483643775E-2</v>
+        <v>1.9487413579535949E-2</v>
       </c>
       <c r="U10" s="2">
         <f t="shared" si="4"/>
-        <v>4.1306677168955613E-4</v>
+        <v>6.8043124830715479E-5</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1">
         <v>6.81</v>
       </c>
       <c r="C11" s="1">
         <v>6.8010000000000002</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
       <c r="R11" s="2">
         <f>F16</f>
-        <v>2.2027697158333331E-2</v>
+        <v>1.7820131704366669E-2</v>
       </c>
       <c r="S11" s="2">
         <f>G16</f>
@@ -4376,15 +3459,15 @@
       </c>
       <c r="T11" s="2">
         <f t="shared" si="3"/>
-        <v>2.1679465960699473E-2</v>
+        <v>1.7896449700667904E-2</v>
       </c>
       <c r="U11" s="2">
         <f t="shared" si="4"/>
-        <v>3.4823119763385812E-4</v>
+        <v>-7.6317996301235314E-5</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="12">
         <v>0.22</v>
       </c>
       <c r="B12" s="1">
@@ -4393,25 +3476,25 @@
       <c r="C12" s="1">
         <v>6.5469999999999997</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="9">
         <f t="shared" ref="D12" si="14">AVERAGE(AVERAGE(B12:B13),AVERAGE(C12:C13))</f>
         <v>6.5514999999999999</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="9">
         <f t="shared" ref="E12" si="15">($J$8/(4*PI()^2))*D12^2</f>
-        <v>1.2876951340359898E-2</v>
-      </c>
-      <c r="F12" s="5">
-        <f t="shared" ref="F12:F25" si="16">A12*$J$3^2+A12*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.3819129352333331E-2</v>
-      </c>
-      <c r="G12" s="5">
+        <v>2.4656691168854508E-2</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" ref="F12:F25" si="16">A12^2*$J$3+A12^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>2.1375431704366666E-2</v>
+      </c>
+      <c r="G12" s="9">
         <f>D12^2</f>
         <v>42.922152249999996</v>
       </c>
       <c r="R12" s="2">
         <f>F18</f>
-        <v>2.1131981061333335E-2</v>
+        <v>1.6169456704366668E-2</v>
       </c>
       <c r="S12" s="2">
         <f>G18</f>
@@ -4419,28 +3502,28 @@
       </c>
       <c r="T12" s="2">
         <f t="shared" si="3"/>
-        <v>2.073102766598918E-2</v>
+        <v>1.6080387070059789E-2</v>
       </c>
       <c r="U12" s="2">
         <f t="shared" si="4"/>
-        <v>4.0095339534415575E-4</v>
+        <v>8.9069634306878503E-5</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="1">
         <v>6.5549999999999997</v>
       </c>
       <c r="C13" s="1">
         <v>6.5490000000000004</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
       <c r="R13" s="2">
         <f>F20</f>
-        <v>2.0236264964333332E-2</v>
+        <v>1.4603431704366664E-2</v>
       </c>
       <c r="S13" s="2">
         <f>G20</f>
@@ -4448,15 +3531,15 @@
       </c>
       <c r="T13" s="2">
         <f t="shared" si="3"/>
-        <v>1.9992840943354798E-2</v>
+        <v>1.4666912594319782E-2</v>
       </c>
       <c r="U13" s="2">
         <f t="shared" si="4"/>
-        <v>2.4342402097853391E-4</v>
+        <v>-6.3480889953117584E-5</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="12">
         <v>0.21</v>
       </c>
       <c r="B14" s="1">
@@ -4465,25 +3548,25 @@
       <c r="C14" s="1">
         <v>6.2919999999999998</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="9">
         <f t="shared" ref="D14" si="17">AVERAGE(AVERAGE(B14:B15),AVERAGE(C14:C15))</f>
         <v>6.2940000000000005</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="9">
         <f t="shared" ref="E14" si="18">($J$8/(4*PI()^2))*D14^2</f>
-        <v>1.1884612909824472E-2</v>
-      </c>
-      <c r="F14" s="5">
-        <f t="shared" ref="F14:F25" si="19">A14*$J$3^2+A14*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.2923413255333331E-2</v>
-      </c>
-      <c r="G14" s="5">
+        <v>2.2756568882921113E-2</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" ref="F14:F25" si="19">A14^2*$J$3+A14^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>1.9555456704366665E-2</v>
+      </c>
+      <c r="G14" s="9">
         <f>D14^2</f>
         <v>39.614436000000005</v>
       </c>
       <c r="R14" s="2">
         <f>F22</f>
-        <v>1.9340548867333336E-2</v>
+        <v>1.3122056704366667E-2</v>
       </c>
       <c r="S14" s="2">
         <f>G22</f>
@@ -4491,28 +3574,28 @@
       </c>
       <c r="T14" s="2">
         <f t="shared" si="3"/>
-        <v>1.9167805140398959E-2</v>
+        <v>1.3087140142049147E-2</v>
       </c>
       <c r="U14" s="2">
         <f t="shared" si="4"/>
-        <v>1.7274372693437678E-4</v>
+        <v>3.4916562317520092E-5</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="1">
         <v>6.298</v>
       </c>
       <c r="C15" s="1">
         <v>6.29</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
       <c r="R15" s="2">
         <f>F24</f>
-        <v>1.4861968382333331E-2</v>
+        <v>6.9849317043666655E-3</v>
       </c>
       <c r="S15" s="2">
         <f>G24</f>
@@ -4520,15 +3603,15 @@
       </c>
       <c r="T15" s="2">
         <f t="shared" si="3"/>
-        <v>1.5989290309467268E-2</v>
+        <v>7.0009434569480531E-3</v>
       </c>
       <c r="U15" s="2">
         <f t="shared" si="4"/>
-        <v>-1.1273219271339362E-3</v>
+        <v>-1.6011752581387637E-5</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16" s="12">
         <v>0.2</v>
       </c>
       <c r="B16" s="1">
@@ -4537,40 +3620,40 @@
       <c r="C16" s="1">
         <v>6.069</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="9">
         <f t="shared" ref="D16" si="20">AVERAGE(AVERAGE(B16:B17),AVERAGE(C16:C17))</f>
         <v>6.07</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="9">
         <f t="shared" ref="E16" si="21">($J$8/(4*PI()^2))*D16^2</f>
-        <v>1.1053732386880169E-2</v>
-      </c>
-      <c r="F16" s="5">
-        <f t="shared" ref="F16:F25" si="22">A16*$J$3^2+A16*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.2027697158333331E-2</v>
-      </c>
-      <c r="G16" s="5">
+        <v>2.1165605004053067E-2</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" ref="F16:F25" si="22">A16^2*$J$3+A16^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>1.7820131704366669E-2</v>
+      </c>
+      <c r="G16" s="9">
         <f>D16^2</f>
         <v>36.844900000000003</v>
       </c>
-      <c r="R16" s="9"/>
+      <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1">
         <v>6.0730000000000004</v>
       </c>
       <c r="C17" s="1">
         <v>6.0659999999999998</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="R17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="12">
         <v>0.19</v>
       </c>
       <c r="B18" s="1">
@@ -4579,39 +3662,39 @@
       <c r="C18" s="1">
         <v>5.8019999999999996</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="9">
         <f t="shared" ref="D18" si="23">AVERAGE(AVERAGE(B18:B19),AVERAGE(C18:C19))</f>
         <v>5.80375</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="9">
         <f t="shared" ref="E18" si="24">($J$8/(4*PI()^2))*D18^2</f>
-        <v>1.0105294092169875E-2</v>
-      </c>
-      <c r="F18" s="5">
-        <f t="shared" ref="F18:F25" si="25">A18*$J$3^2+A18*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.1131981061333335E-2</v>
-      </c>
-      <c r="G18" s="5">
+        <v>1.9349542373444953E-2</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" ref="F18:F25" si="25">A18^2*$J$3+A18^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>1.6169456704366668E-2</v>
+      </c>
+      <c r="G18" s="9">
         <f>D18^2</f>
         <v>33.683514062500002</v>
       </c>
-      <c r="R18" s="9"/>
+      <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="1">
         <v>5.8070000000000004</v>
       </c>
       <c r="C19" s="1">
         <v>5.7990000000000004</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20" s="12">
         <v>0.18</v>
       </c>
       <c r="B20" s="1">
@@ -4620,38 +3703,38 @@
       <c r="C20" s="1">
         <v>5.5839999999999996</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="9">
         <f t="shared" ref="D20" si="26">AVERAGE(AVERAGE(B20:B21),AVERAGE(C20:C21))</f>
         <v>5.5877499999999998</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="9">
         <f t="shared" ref="E20" si="27">($J$8/(4*PI()^2))*D20^2</f>
-        <v>9.3671073695354955E-3</v>
-      </c>
-      <c r="F20" s="5">
-        <f t="shared" ref="F20:F25" si="28">A20*$J$3^2+A20*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>2.0236264964333332E-2</v>
-      </c>
-      <c r="G20" s="5">
+        <v>1.7936067897704945E-2</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" ref="F20:F25" si="28">A20^2*$J$3+A20^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>1.4603431704366664E-2</v>
+      </c>
+      <c r="G20" s="9">
         <f>D20^2</f>
         <v>31.222950062499997</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="1">
         <v>5.5919999999999996</v>
       </c>
       <c r="C21" s="1">
         <v>5.5839999999999996</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22" s="12">
         <v>0.17</v>
       </c>
       <c r="B22" s="1">
@@ -4660,38 +3743,38 @@
       <c r="C22" s="1">
         <v>5.3310000000000004</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="9">
         <f t="shared" ref="D22" si="29">AVERAGE(AVERAGE(B22:B23),AVERAGE(C22:C23))</f>
         <v>5.3360000000000003</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="9">
         <f t="shared" ref="E22" si="30">($J$8/(4*PI()^2))*D22^2</f>
-        <v>8.5420715665796565E-3</v>
-      </c>
-      <c r="F22" s="5">
-        <f t="shared" ref="F22:F25" si="31">A22*$J$3^2+A22*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>1.9340548867333336E-2</v>
-      </c>
-      <c r="G22" s="5">
+        <v>1.6356295445434311E-2</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" ref="F22:F25" si="31">A22^2*$J$3+A22^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>1.3122056704366667E-2</v>
+      </c>
+      <c r="G22" s="9">
         <f>D22^2</f>
         <v>28.472896000000002</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="1">
         <v>5.343</v>
       </c>
       <c r="C23" s="1">
         <v>5.3310000000000004</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="A24" s="12">
         <v>0.12</v>
       </c>
       <c r="B24" s="1">
@@ -4700,77 +3783,50 @@
       <c r="C24" s="1">
         <v>4.2249999999999996</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="9">
         <f t="shared" ref="D24" si="32">AVERAGE(AVERAGE(B24:B25),AVERAGE(C24:C25))</f>
         <v>4.2282499999999992</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="9">
         <f t="shared" ref="E24" si="33">($J$8/(4*PI()^2))*D24^2</f>
-        <v>5.3635567356479664E-3</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" ref="F24:F25" si="34">A24*$J$3^2+A24*$J$4^2+($J$5*$J$6^2)/12</f>
-        <v>1.4861968382333331E-2</v>
-      </c>
-      <c r="G24" s="5">
+        <v>1.0270098760333217E-2</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" ref="F24:F25" si="34">A24^2*$J$3+A24^2*$J$4+($J$5^2*$J$6)/12</f>
+        <v>6.9849317043666655E-3</v>
+      </c>
+      <c r="G24" s="9">
         <f>D24^2</f>
         <v>17.878098062499994</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="1">
         <v>4.2309999999999999</v>
       </c>
       <c r="C25" s="1">
         <v>4.2240000000000002</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="G14:G15"/>
@@ -4781,18 +3837,45 @@
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="G20:G21"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G10:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4802,20 +3885,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322AEA10-24EE-40F7-8525-64347259AD68}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="8" width="8.88671875" style="2"/>
-    <col min="9" max="9" width="11.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -4835,25 +3918,25 @@
         <v>2</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <f>B2-$P$2</f>
+        <f>B2-$O$2</f>
         <v>0.11049999999999999</v>
       </c>
       <c r="B2" s="1">
-        <f>$N$5-C2</f>
+        <f>$M$5-C2</f>
         <v>0.376</v>
       </c>
       <c r="C2" s="1">
@@ -4866,49 +3949,45 @@
         <v>7.5949999999999998</v>
       </c>
       <c r="F2" s="1">
-        <f>(D2+E2)/2</f>
+        <f>AVERAGE(D2:E2)</f>
         <v>7.5990000000000002</v>
       </c>
       <c r="G2" s="1">
-        <f>('d1 == d2'!$J$8/(4*PI()^2))*F2^2</f>
-        <v>1.7323851523213533E-2</v>
-      </c>
-      <c r="H2" s="1">
-        <f>B2*$N$2^2+C2*$N$3^2+($N$4*$N$5^2)/12</f>
-        <v>3.1526139755433336E-2</v>
-      </c>
-      <c r="I2" s="1">
-        <f>ABS(G2-H2)/H2*100</f>
-        <v>45.049245934945539</v>
-      </c>
-      <c r="J2" s="1">
         <f>F2^2</f>
         <v>57.744801000000002</v>
       </c>
-      <c r="K2" s="2">
-        <f>G2+($N$2+$N$3+$N$4)*A2^2</f>
-        <v>2.4106279090713532E-2</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="H2" s="1">
+        <f>'d1 == d2'!J$8*G2/(4*PI()*PI())</f>
+        <v>3.3171582742893821E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <f>M$7+O$4*A2^2</f>
+        <v>4.0730801098333332E-2</v>
+      </c>
+      <c r="J2" s="6">
+        <f>ABS(I2-H2)/I2</f>
+        <v>0.18558972943325749</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
         <v>0.21243999999999999</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="1">
+      <c r="O2" s="1">
         <v>0.26550000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A8" si="0">B3-$P$2</f>
+        <f>B3-$O$2</f>
         <v>0.1255</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B8" si="1">$N$5-C3</f>
+        <f>$M$5-C3</f>
         <v>0.39100000000000001</v>
       </c>
       <c r="C3" s="1">
@@ -4921,49 +4000,45 @@
         <v>7.5519999999999996</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F8" si="2">(D3+E3)/2</f>
+        <f t="shared" ref="F3:F8" si="0">AVERAGE(D3:E3)</f>
         <v>7.5564999999999998</v>
       </c>
       <c r="G3" s="1">
-        <f>('d1 == d2'!$J$8/(4*PI()^2))*F3^2</f>
-        <v>1.7130614311264308E-2</v>
-      </c>
-      <c r="H3" s="1">
-        <f t="shared" ref="H3:H8" si="3">B3*$N$2^2+C3*$N$3^2+($N$4*$N$5^2)/12</f>
-        <v>3.1536488217933333E-2</v>
-      </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I8" si="4">ABS(G3-H3)/H3*100</f>
-        <v>45.680019306896305</v>
-      </c>
-      <c r="J3" s="1">
         <f>F3^2</f>
         <v>57.100692249999994</v>
       </c>
-      <c r="K3" s="2">
-        <f t="shared" ref="K3:K8" si="5">G3+($N$2+$N$3+$N$4)*A3^2</f>
-        <v>2.587940567876431E-2</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="H3" s="1">
+        <f>'d1 == d2'!J$8*G3/(4*PI()*PI())</f>
+        <v>3.2801573558932005E-2</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I8" si="1">M$7+O$4*A3^2</f>
+        <v>4.2697164898333334E-2</v>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" ref="J3:J8" si="2">ABS(I3-H3)/I3</f>
+        <v>0.23176225782118848</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="1">
+      <c r="M3" s="1">
         <v>0.21081</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="1">
+      <c r="O3" s="1">
         <v>0.26550000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f t="shared" si="0"/>
+        <f>B4-$O$2</f>
         <v>0.13550000000000001</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="1"/>
+        <f>$M$5-C4</f>
         <v>0.40100000000000002</v>
       </c>
       <c r="C4" s="1">
@@ -4976,43 +4051,46 @@
         <v>7.5309999999999997</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.5339999999999998</v>
       </c>
       <c r="G4" s="1">
-        <f>('d1 == d2'!$J$8/(4*PI()^2))*F4^2</f>
-        <v>1.7028751018294458E-2</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1543387192933335E-2</v>
-      </c>
-      <c r="I4" s="1">
-        <f t="shared" si="4"/>
-        <v>46.014830575616152</v>
-      </c>
-      <c r="J4" s="1">
         <f>F4^2</f>
         <v>56.761156</v>
       </c>
-      <c r="K4" s="2">
-        <f t="shared" si="5"/>
-        <v>2.7227319085794462E-2</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="H4" s="1">
+        <f>'d1 == d2'!J$8*G4/(4*PI()*PI())</f>
+        <v>3.2606526479090368E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="1"/>
+        <v>4.4146941598333336E-2</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" si="2"/>
+        <v>0.26140916451794816</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="1">
+      <c r="M4" s="1">
         <v>0.13222</v>
       </c>
+      <c r="N4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1">
+        <f>M2+M3+M4</f>
+        <v>0.55547000000000002</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
+        <f>B5-$O$2</f>
         <v>0.14549999999999996</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="1"/>
+        <f>$M$5-C5</f>
         <v>0.41099999999999998</v>
       </c>
       <c r="C5" s="1">
@@ -5025,43 +4103,39 @@
         <v>7.53</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.5355000000000008</v>
       </c>
       <c r="G5" s="1">
-        <f>('d1 == d2'!$J$8/(4*PI()^2))*F5^2</f>
-        <v>1.7035532454268129E-2</v>
-      </c>
-      <c r="H5" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1550286167933331E-2</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="4"/>
-        <v>46.005141241531803</v>
-      </c>
-      <c r="J5" s="1">
         <f>F5^2</f>
         <v>56.783760250000014</v>
       </c>
-      <c r="K5" s="2">
-        <f t="shared" si="5"/>
-        <v>2.879497122176812E-2</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="H5" s="1">
+        <f>'d1 == d2'!J$8*G5/(4*PI()*PI())</f>
+        <v>3.2619511522526859E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5707812298333324E-2</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" si="2"/>
+        <v>0.28634712793470785</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="1">
+      <c r="M5" s="1">
         <v>0.61099999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f>B6-$O$2</f>
         <v>0.15549999999999997</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="1"/>
+        <f>$M$5-C6</f>
         <v>0.42099999999999999</v>
       </c>
       <c r="C6" s="1">
@@ -5074,37 +4148,33 @@
         <v>7.532</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.5380000000000003</v>
       </c>
       <c r="G6" s="1">
-        <f>('d1 == d2'!$J$8/(4*PI()^2))*F6^2</f>
-        <v>1.7046837847628785E-2</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1557185142933333E-2</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" si="4"/>
-        <v>45.981120399624366</v>
-      </c>
-      <c r="J6" s="1">
         <f>F6^2</f>
         <v>56.821444000000007</v>
       </c>
-      <c r="K6" s="2">
-        <f t="shared" si="5"/>
-        <v>3.047824131512878E-2</v>
+      <c r="H6" s="1">
+        <f>'d1 == d2'!J$8*G6/(4*PI()*PI())</f>
+        <v>3.2641159006101823E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7379776998333331E-2</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="2"/>
+        <v>0.31107402621903363</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f>B7-$O$2</f>
         <v>0.16549999999999998</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="1"/>
+        <f>$M$5-C7</f>
         <v>0.43099999999999999</v>
       </c>
       <c r="C7" s="1">
@@ -5117,37 +4187,40 @@
         <v>7.524</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.5350000000000001</v>
       </c>
       <c r="G7" s="1">
-        <f>('d1 == d2'!$J$8/(4*PI()^2))*F7^2</f>
-        <v>1.7033271825606676E-2</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1564084117933336E-2</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="4"/>
-        <v>46.035906627402781</v>
-      </c>
-      <c r="J7" s="1">
         <f>F7^2</f>
         <v>56.776225000000004</v>
       </c>
-      <c r="K7" s="2">
-        <f t="shared" si="5"/>
-        <v>3.2247733993106674E-2</v>
+      <c r="H7" s="1">
+        <f>'d1 == d2'!J$8*G7/(4*PI()*PI())</f>
+        <v>3.2615182887488985E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9162835698333331E-2</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="2"/>
+        <v>0.33658865636599816</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="1">
+        <f>M2*O2^2+M3*O3^2+M4*M5^2/12</f>
+        <v>3.3948373530833333E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f>B8-$O$2</f>
         <v>0.17549999999999993</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="1"/>
+        <f>$M$5-C8</f>
         <v>0.44099999999999995</v>
       </c>
       <c r="C8" s="1">
@@ -5160,33 +4233,31 @@
         <v>7.5460000000000003</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.5660000000000007</v>
       </c>
       <c r="G8" s="1">
-        <f>('d1 == d2'!$J$8/(4*PI()^2))*F8^2</f>
-        <v>1.7173714459349818E-2</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1570983092933325E-2</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="4"/>
-        <v>45.602851806050069</v>
-      </c>
-      <c r="J8" s="1">
         <f>F8^2</f>
         <v>57.24435600000001</v>
       </c>
-      <c r="K8" s="2">
-        <f t="shared" si="5"/>
-        <v>3.4282329326849804E-2</v>
+      <c r="H8" s="1">
+        <f>'d1 == d2'!J$8*G8/(4*PI()*PI())</f>
+        <v>3.2884101403651396E-2</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>5.1056988398333322E-2</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.355933390604667</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5194,7 +4265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C7C9C7-DDA4-41C1-9791-3ACEA0C01E4B}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -5224,11 +4295,11 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="5">
+      <c r="D2" s="9">
         <f>(B2+C2)/2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="9"/>
       <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
@@ -5238,43 +4309,43 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>